<commit_message>
03 MAR / 14:00
</commit_message>
<xml_diff>
--- a/04.Tablas/Info_ppt.xlsx
+++ b/04.Tablas/Info_ppt.xlsx
@@ -10,8 +10,8 @@
     <sheet name="Horiz.Pred" sheetId="3" r:id="rId1"/>
     <sheet name="Fig.RN" sheetId="4" r:id="rId2"/>
     <sheet name="Log.Conv" sheetId="5" r:id="rId3"/>
-    <sheet name="Arq.RN" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
+    <sheet name="Arq.RN" sheetId="7" r:id="rId4"/>
+    <sheet name="Ejecucón" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="81">
   <si>
     <t>Muy Corto Plazo</t>
   </si>
@@ -159,13 +159,132 @@
   </si>
   <si>
     <t>R profunda</t>
+  </si>
+  <si>
+    <t>LSTM</t>
+  </si>
+  <si>
+    <t>R^2</t>
+  </si>
+  <si>
+    <t>0,31</t>
+  </si>
+  <si>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>0,324</t>
+  </si>
+  <si>
+    <t>0,322</t>
+  </si>
+  <si>
+    <t>0,311</t>
+  </si>
+  <si>
+    <t>0,325</t>
+  </si>
+  <si>
+    <t>0,03</t>
+  </si>
+  <si>
+    <t>0,297</t>
+  </si>
+  <si>
+    <t>0,321</t>
+  </si>
+  <si>
+    <t>0,323</t>
+  </si>
+  <si>
+    <t>0,312</t>
+  </si>
+  <si>
+    <t>0,286</t>
+  </si>
+  <si>
+    <t>Epocas</t>
+  </si>
+  <si>
+    <t>Red Simple</t>
+  </si>
+  <si>
+    <t>Red Profunda</t>
+  </si>
+  <si>
+    <t>Capas
+Ocultas</t>
+  </si>
+  <si>
+    <t>Neuronas</t>
+  </si>
+  <si>
+    <t>0,26</t>
+  </si>
+  <si>
+    <t>0,0283</t>
+  </si>
+  <si>
+    <t>0,0287</t>
+  </si>
+  <si>
+    <t>0,24</t>
+  </si>
+  <si>
+    <t>0,0294</t>
+  </si>
+  <si>
+    <t>0,0285</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>0,0286</t>
+  </si>
+  <si>
+    <t>0,27</t>
+  </si>
+  <si>
+    <t>0,0284</t>
+  </si>
+  <si>
+    <t>0,271</t>
+  </si>
+  <si>
+    <t>0,269</t>
+  </si>
+  <si>
+    <t>0,272</t>
+  </si>
+  <si>
+    <t>0,33</t>
+  </si>
+  <si>
+    <t>0,32</t>
+  </si>
+  <si>
+    <t>0,0282</t>
+  </si>
+  <si>
+    <t>0,274</t>
+  </si>
+  <si>
+    <t>0,0281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R^2 Keras </t>
+  </si>
+  <si>
+    <t>Error minimo 
+cuadrado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,8 +349,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +392,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -345,7 +477,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -405,8 +537,132 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -452,6 +708,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -464,11 +732,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -498,6 +775,68 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -527,6 +866,68 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1728,23 +2129,7 @@
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Direcci</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>ón </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>del Viento</a:t>
+            <a:t>Dirección del Viento</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -1977,21 +2362,8 @@
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Energ</a:t>
+            <a:t>Energía Generada</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>ía Generada</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr algn="ctr"/>
@@ -2341,23 +2713,7 @@
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Direcci</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>ón </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>del Viento</a:t>
+            <a:t>Dirección del Viento</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -2395,14 +2751,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2411,8 +2767,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11506200" y="800100"/>
-          <a:ext cx="1092200" cy="2146300"/>
+          <a:off x="11506200" y="1054100"/>
+          <a:ext cx="1092200" cy="1612900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2448,14 +2804,6 @@
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -2510,7 +2858,7 @@
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>100 neuronas</a:t>
+            <a:t>50 neuronas</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -2590,21 +2938,8 @@
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Energ</a:t>
+            <a:t>Energía Generada</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>ía Generada</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr algn="ctr"/>
@@ -2689,7 +3024,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>177800</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
@@ -2706,9 +3041,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10909300" y="1873250"/>
-          <a:ext cx="596900" cy="0"/>
+        <a:xfrm flipV="1">
+          <a:off x="10909300" y="1860550"/>
+          <a:ext cx="596900" cy="12700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2862,7 +3197,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
@@ -2880,8 +3215,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12598400" y="1873250"/>
-          <a:ext cx="571500" cy="0"/>
+          <a:off x="12598400" y="1860550"/>
+          <a:ext cx="571500" cy="12700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2932,6 +3267,771 @@
         <a:xfrm>
           <a:off x="14262100" y="1873250"/>
           <a:ext cx="609600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rectangle 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18694400" y="736600"/>
+          <a:ext cx="1104900" cy="939800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Velocidad del Viento</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(ws)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1 neurona</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="Rectangle 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18681700" y="1955800"/>
+          <a:ext cx="1104900" cy="927100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Dirección del Viento</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(wd)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1 neurona</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Rectangle 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20624800" y="762000"/>
+          <a:ext cx="1092200" cy="2146300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Capa</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Oculta #1 </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>100 neuronas</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Rectangle 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23990300" y="1295400"/>
+          <a:ext cx="1104900" cy="1079500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Energía Generada</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(wp1)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1 neurona</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Right Bracket 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19799300" y="1193800"/>
+          <a:ext cx="228600" cy="1282700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBracket">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Connector 40"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="40" idx="2"/>
+          <a:endCxn id="38" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20027900" y="1835150"/>
+          <a:ext cx="596900" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Rectangle 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22288500" y="774700"/>
+          <a:ext cx="1092200" cy="2146300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Capa</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Oculta #2 </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>100 neuronas</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Connector 42"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="38" idx="3"/>
+          <a:endCxn id="42" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21717000" y="1835150"/>
+          <a:ext cx="571500" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="42" idx="3"/>
+          <a:endCxn id="39" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="23380700" y="1835150"/>
+          <a:ext cx="609600" cy="12700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3215,7 +4315,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3565,7 +4665,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="23" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="7"/>
@@ -3579,7 +4679,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="17"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="2:9">
@@ -3646,7 +4746,7 @@
   <dimension ref="B3:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3694,7 +4794,7 @@
       <c r="C4" s="12">
         <v>1</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="24">
         <v>0</v>
       </c>
       <c r="E4" s="12" t="s">
@@ -3720,7 +4820,7 @@
       <c r="C5" s="12">
         <v>27</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="12" t="s">
         <v>34</v>
       </c>
@@ -3744,7 +4844,7 @@
       <c r="C6" s="12">
         <v>1</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="24">
         <v>12</v>
       </c>
       <c r="E6" s="12" t="s">
@@ -3770,7 +4870,7 @@
       <c r="C7" s="12">
         <v>27</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="12" t="s">
         <v>36</v>
       </c>
@@ -3794,7 +4894,7 @@
       <c r="C8" s="12">
         <v>40</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="12" t="s">
         <v>37</v>
       </c>
@@ -3828,13 +4928,623 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:AF21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="22" max="22" width="6.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:32">
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+    </row>
+    <row r="2" spans="2:32">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+    </row>
+    <row r="3" spans="2:32">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+    </row>
+    <row r="4" spans="2:32">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+    </row>
+    <row r="5" spans="2:32">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+    </row>
+    <row r="6" spans="2:32">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+    </row>
+    <row r="7" spans="2:32">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+    </row>
+    <row r="8" spans="2:32">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+    </row>
+    <row r="9" spans="2:32">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+    </row>
+    <row r="10" spans="2:32">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+    </row>
+    <row r="11" spans="2:32">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+    </row>
+    <row r="12" spans="2:32">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+    </row>
+    <row r="13" spans="2:32">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+    </row>
+    <row r="14" spans="2:32">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+    </row>
+    <row r="15" spans="2:32">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+    </row>
+    <row r="16" spans="2:32">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+    </row>
+    <row r="17" spans="2:32">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+    </row>
+    <row r="18" spans="2:32">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+    </row>
+    <row r="19" spans="2:32">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+    </row>
+    <row r="20" spans="2:32">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+    </row>
+    <row r="21" spans="2:32">
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3845,418 +5555,966 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U21"/>
+  <dimension ref="B2:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:21">
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-    </row>
-    <row r="2" spans="2:21">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-    </row>
-    <row r="3" spans="2:21">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+    <row r="2" spans="2:22">
+      <c r="E2" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="J2" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+    </row>
+    <row r="3" spans="2:22">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
       <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-    </row>
-    <row r="4" spans="2:21">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-    </row>
-    <row r="5" spans="2:21">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-    </row>
-    <row r="6" spans="2:21">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-    </row>
-    <row r="7" spans="2:21">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-    </row>
-    <row r="8" spans="2:21">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-    </row>
-    <row r="9" spans="2:21">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-    </row>
-    <row r="10" spans="2:21">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-    </row>
-    <row r="11" spans="2:21">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-    </row>
-    <row r="12" spans="2:21">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-    </row>
-    <row r="13" spans="2:21">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-    </row>
-    <row r="14" spans="2:21">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-    </row>
-    <row r="15" spans="2:21">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-    </row>
-    <row r="16" spans="2:21">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-    </row>
-    <row r="17" spans="2:21">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-    </row>
-    <row r="18" spans="2:21">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-    </row>
-    <row r="19" spans="2:21">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-    </row>
-    <row r="20" spans="2:21">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-    </row>
-    <row r="21" spans="2:21">
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
+    </row>
+    <row r="4" spans="2:22" ht="24">
+      <c r="B4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22">
+      <c r="B5" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="21">
+        <v>50</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="21">
+        <v>13</v>
+      </c>
+      <c r="J5" s="28">
+        <v>50</v>
+      </c>
+      <c r="K5" s="28">
+        <v>2</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="28">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="28">
+        <v>50</v>
+      </c>
+      <c r="R5" s="28">
+        <v>2</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="V5" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22">
+      <c r="E6" s="21">
+        <v>80</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="21">
+        <v>13</v>
+      </c>
+      <c r="J6" s="28">
+        <v>50</v>
+      </c>
+      <c r="K6" s="28">
+        <v>4</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" s="28">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="28">
+        <v>50</v>
+      </c>
+      <c r="R6" s="28">
+        <v>4</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="U6" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22">
+      <c r="E7" s="21">
+        <v>100</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="21">
+        <v>13</v>
+      </c>
+      <c r="J7" s="28">
+        <v>50</v>
+      </c>
+      <c r="K7" s="28">
+        <v>6</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="O7" s="28">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="28">
+        <v>50</v>
+      </c>
+      <c r="R7" s="28">
+        <v>6</v>
+      </c>
+      <c r="S7" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="T7" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="U7" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22">
+      <c r="E8" s="21">
+        <v>120</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="21">
+        <v>13</v>
+      </c>
+      <c r="J8" s="28">
+        <v>50</v>
+      </c>
+      <c r="K8" s="28">
+        <v>8</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="28">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="28">
+        <v>50</v>
+      </c>
+      <c r="R8" s="28">
+        <v>8</v>
+      </c>
+      <c r="S8" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="T8" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="U8" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="V8" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22">
+      <c r="E9" s="21">
+        <v>140</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="21">
+        <v>13</v>
+      </c>
+      <c r="J9" s="28">
+        <v>50</v>
+      </c>
+      <c r="K9" s="28">
+        <v>2</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="O9" s="28">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="28">
+        <v>50</v>
+      </c>
+      <c r="R9" s="28">
+        <v>2</v>
+      </c>
+      <c r="S9" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="T9" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="U9" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22">
+      <c r="E10" s="21">
+        <v>160</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="21">
+        <v>13</v>
+      </c>
+      <c r="J10" s="28">
+        <v>50</v>
+      </c>
+      <c r="K10" s="28">
+        <v>4</v>
+      </c>
+      <c r="L10" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="O10" s="28">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="28">
+        <v>50</v>
+      </c>
+      <c r="R10" s="28">
+        <v>4</v>
+      </c>
+      <c r="S10" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="T10" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="U10" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="V10" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22">
+      <c r="E11" s="21">
+        <v>180</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="21">
+        <v>13</v>
+      </c>
+      <c r="J11" s="28">
+        <v>50</v>
+      </c>
+      <c r="K11" s="28">
+        <v>6</v>
+      </c>
+      <c r="L11" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" s="28">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="28">
+        <v>50</v>
+      </c>
+      <c r="R11" s="28">
+        <v>6</v>
+      </c>
+      <c r="S11" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="T11" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U11" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="V11" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22">
+      <c r="E12" s="29">
+        <v>200</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="30">
+        <v>13</v>
+      </c>
+      <c r="J12" s="28">
+        <v>50</v>
+      </c>
+      <c r="K12" s="28">
+        <v>8</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N12" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="O12" s="28">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="28">
+        <v>50</v>
+      </c>
+      <c r="R12" s="28">
+        <v>8</v>
+      </c>
+      <c r="S12" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="T12" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U12" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="V12" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22">
+      <c r="E13" s="28">
+        <v>220</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="28">
+        <v>13</v>
+      </c>
+      <c r="J13" s="28">
+        <v>50</v>
+      </c>
+      <c r="K13" s="28">
+        <v>4</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="M13" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N13" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="28">
+        <v>25</v>
+      </c>
+      <c r="Q13" s="28">
+        <v>50</v>
+      </c>
+      <c r="R13" s="28">
+        <v>4</v>
+      </c>
+      <c r="S13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T13" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U13" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="V13" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22">
+      <c r="E14" s="28">
+        <v>240</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="28">
+        <v>13</v>
+      </c>
+      <c r="J14" s="28">
+        <v>50</v>
+      </c>
+      <c r="K14" s="28">
+        <v>6</v>
+      </c>
+      <c r="L14" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="M14" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="N14" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="O14" s="28">
+        <v>25</v>
+      </c>
+      <c r="Q14" s="28">
+        <v>50</v>
+      </c>
+      <c r="R14" s="28">
+        <v>6</v>
+      </c>
+      <c r="S14" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="T14" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="U14" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="V14" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22">
+      <c r="E15" s="28">
+        <v>260</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="28">
+        <v>13</v>
+      </c>
+      <c r="J15" s="29">
+        <v>100</v>
+      </c>
+      <c r="K15" s="29">
+        <v>4</v>
+      </c>
+      <c r="L15" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="N15" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" s="29">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="29">
+        <v>100</v>
+      </c>
+      <c r="R15" s="29">
+        <v>4</v>
+      </c>
+      <c r="S15" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="T15" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U15" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="V15" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22">
+      <c r="E16" s="28">
+        <v>300</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="28">
+        <v>13</v>
+      </c>
+      <c r="J16" s="28">
+        <v>100</v>
+      </c>
+      <c r="K16" s="28">
+        <v>6</v>
+      </c>
+      <c r="L16" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="M16" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="N16" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="O16" s="28">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="28">
+        <v>100</v>
+      </c>
+      <c r="R16" s="28">
+        <v>6</v>
+      </c>
+      <c r="S16" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="T16" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="U16" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="V16" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="5:22">
+      <c r="E17" s="28">
+        <v>400</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="28">
+        <v>13</v>
+      </c>
+      <c r="J17" s="28">
+        <v>100</v>
+      </c>
+      <c r="K17" s="28">
+        <v>4</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="M17" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N17" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="O17" s="28">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="28">
+        <v>100</v>
+      </c>
+      <c r="R17" s="28">
+        <v>4</v>
+      </c>
+      <c r="S17" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T17" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U17" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="V17" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="5:22">
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="J18" s="28">
+        <v>100</v>
+      </c>
+      <c r="K18" s="28">
+        <v>6</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="M18" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N18" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="O18" s="28">
+        <v>25</v>
+      </c>
+      <c r="Q18" s="28">
+        <v>100</v>
+      </c>
+      <c r="R18" s="28">
+        <v>6</v>
+      </c>
+      <c r="S18" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="T18" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U18" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="V18" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="5:22">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="J19" s="28">
+        <v>200</v>
+      </c>
+      <c r="K19" s="28">
+        <v>4</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N19" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="O19" s="28">
+        <v>20</v>
+      </c>
+      <c r="Q19" s="28">
+        <v>200</v>
+      </c>
+      <c r="R19" s="28">
+        <v>4</v>
+      </c>
+      <c r="S19" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T19" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U19" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="V19" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="5:22">
+      <c r="J20" s="28">
+        <v>200</v>
+      </c>
+      <c r="K20" s="28">
+        <v>6</v>
+      </c>
+      <c r="L20" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="M20" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N20" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="O20" s="28">
+        <v>25</v>
+      </c>
+      <c r="Q20" s="28">
+        <v>200</v>
+      </c>
+      <c r="R20" s="28">
+        <v>6</v>
+      </c>
+      <c r="S20" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="T20" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U20" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="V20" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="5:22">
+      <c r="J21" s="28">
+        <v>300</v>
+      </c>
+      <c r="K21" s="28">
+        <v>4</v>
+      </c>
+      <c r="L21" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="M21" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N21" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="O21" s="28">
+        <v>20</v>
+      </c>
+      <c r="Q21" s="28">
+        <v>300</v>
+      </c>
+      <c r="R21" s="28">
+        <v>4</v>
+      </c>
+      <c r="S21" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="T21" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U21" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="V21" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="5:22">
+      <c r="J22" s="28">
+        <v>400</v>
+      </c>
+      <c r="K22" s="28">
+        <v>4</v>
+      </c>
+      <c r="L22" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="M22" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N22" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="O22" s="28">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="28">
+        <v>400</v>
+      </c>
+      <c r="R22" s="28">
+        <v>4</v>
+      </c>
+      <c r="S22" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T22" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U22" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="V22" s="28">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="J2:O2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
03 MAR / 23:30
03 MAR / 23:30
</commit_message>
<xml_diff>
--- a/04.Tablas/Info_ppt.xlsx
+++ b/04.Tablas/Info_ppt.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="92">
   <si>
     <t>Muy Corto Plazo</t>
   </si>
@@ -278,6 +278,39 @@
   <si>
     <t>Error minimo 
 cuadrado</t>
+  </si>
+  <si>
+    <t>Red LSTM</t>
+  </si>
+  <si>
+    <t>0,0288</t>
+  </si>
+  <si>
+    <t>0,0422</t>
+  </si>
+  <si>
+    <t>0,34</t>
+  </si>
+  <si>
+    <t>0,0325</t>
+  </si>
+  <si>
+    <t>0,28</t>
+  </si>
+  <si>
+    <t>Modelo ML</t>
+  </si>
+  <si>
+    <t>0,0280</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Reg Lineal</t>
+  </si>
+  <si>
+    <t>Red Neu. Simple</t>
   </si>
 </sst>
 </file>
@@ -477,7 +510,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -661,8 +694,50 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -744,8 +819,14 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="225">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -837,6 +918,27 @@
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -928,6 +1030,27 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5555,10 +5678,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V22"/>
+  <dimension ref="B2:AB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5570,9 +5693,11 @@
     <col min="13" max="13" width="4.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.83203125" customWidth="1"/>
+    <col min="26" max="26" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22">
+    <row r="2" spans="2:28">
       <c r="E2" s="27" t="s">
         <v>57</v>
       </c>
@@ -5587,8 +5712,15 @@
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
       <c r="O2" s="27"/>
-    </row>
-    <row r="3" spans="2:22">
+      <c r="Q2" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+    </row>
+    <row r="3" spans="2:28">
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
@@ -5600,7 +5732,7 @@
       <c r="N3" s="22"/>
       <c r="O3" s="22"/>
     </row>
-    <row r="4" spans="2:22" ht="24">
+    <row r="4" spans="2:28" ht="24">
       <c r="B4" s="11" t="s">
         <v>43</v>
       </c>
@@ -5644,23 +5776,38 @@
         <v>59</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="T4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="X4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="11" t="s">
+      <c r="AA4" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="V4" s="11" t="s">
+      <c r="AB4" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:22">
-      <c r="B5" s="28" t="s">
+    <row r="5" spans="2:28">
+      <c r="B5" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="30" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="21">
@@ -5694,25 +5841,42 @@
         <v>10</v>
       </c>
       <c r="Q5" s="28">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="R5" s="28">
         <v>2</v>
       </c>
       <c r="S5" s="28" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="T5" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="U5" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="V5" s="28">
+        <v>68</v>
+      </c>
+      <c r="U5" s="28">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="2:22">
+      <c r="W5" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="X5" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y5" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z5" s="28" t="str">
+        <f>B5</f>
+        <v>0,32</v>
+      </c>
+      <c r="AA5" s="28" t="str">
+        <f>C5</f>
+        <v>0,03</v>
+      </c>
+      <c r="AB5" s="28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28">
       <c r="E6" s="21">
         <v>80</v>
       </c>
@@ -5744,25 +5908,44 @@
         <v>10</v>
       </c>
       <c r="Q6" s="28">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="R6" s="28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S6" s="28" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="T6" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="U6" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V6" s="28">
+        <v>66</v>
+      </c>
+      <c r="U6" s="28">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="2:22">
+      <c r="W6" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="X6" s="28">
+        <f>E12</f>
+        <v>200</v>
+      </c>
+      <c r="Y6" s="28">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="28" t="str">
+        <f>F12</f>
+        <v>0,325</v>
+      </c>
+      <c r="AA6" s="28" t="str">
+        <f>G12</f>
+        <v>0,03</v>
+      </c>
+      <c r="AB6" s="28">
+        <f>H12</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28">
       <c r="E7" s="21">
         <v>100</v>
       </c>
@@ -5794,25 +5977,45 @@
         <v>10</v>
       </c>
       <c r="Q7" s="28">
+        <v>100</v>
+      </c>
+      <c r="R7" s="28">
+        <v>10</v>
+      </c>
+      <c r="S7" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="T7" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="U7" s="28">
+        <v>10</v>
+      </c>
+      <c r="W7" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="X7" s="28">
+        <f>J11</f>
         <v>50</v>
       </c>
-      <c r="R7" s="28">
+      <c r="Y7" s="28">
+        <f>K11</f>
         <v>6</v>
       </c>
-      <c r="S7" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="T7" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="U7" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V7" s="28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22">
+      <c r="Z7" s="28" t="str">
+        <f>M11</f>
+        <v>0,33</v>
+      </c>
+      <c r="AA7" s="28" t="str">
+        <f>N11</f>
+        <v>0,0282</v>
+      </c>
+      <c r="AB7" s="28">
+        <f>O11</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28">
       <c r="E8" s="21">
         <v>120</v>
       </c>
@@ -5844,25 +6047,45 @@
         <v>10</v>
       </c>
       <c r="Q8" s="28">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="R8" s="28">
-        <v>8</v>
-      </c>
-      <c r="S8" s="28" t="s">
-        <v>67</v>
+        <v>20</v>
+      </c>
+      <c r="S8" s="28">
+        <v>0</v>
       </c>
       <c r="T8" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="U8" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="V8" s="28">
+        <v>83</v>
+      </c>
+      <c r="U8" s="28">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:22">
+      <c r="W8" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="X8" s="28">
+        <f>Q14</f>
+        <v>100</v>
+      </c>
+      <c r="Y8" s="28">
+        <f>R14</f>
+        <v>5</v>
+      </c>
+      <c r="Z8" s="28" t="str">
+        <f>S14</f>
+        <v>0,34</v>
+      </c>
+      <c r="AA8" s="28" t="str">
+        <f>T14</f>
+        <v>0,0280</v>
+      </c>
+      <c r="AB8" s="28">
+        <f>U14</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28">
       <c r="E9" s="21">
         <v>140</v>
       </c>
@@ -5894,25 +6117,22 @@
         <v>20</v>
       </c>
       <c r="Q9" s="28">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="R9" s="28">
         <v>2</v>
       </c>
       <c r="S9" s="28" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="T9" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="U9" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V9" s="28">
+        <v>78</v>
+      </c>
+      <c r="U9" s="28">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:22">
+    <row r="10" spans="2:28">
       <c r="E10" s="21">
         <v>160</v>
       </c>
@@ -5944,25 +6164,22 @@
         <v>20</v>
       </c>
       <c r="Q10" s="28">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="R10" s="28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S10" s="28" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="T10" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="U10" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="V10" s="28">
+        <v>88</v>
+      </c>
+      <c r="U10" s="28">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:22">
+    <row r="11" spans="2:28">
       <c r="E11" s="21">
         <v>180</v>
       </c>
@@ -5975,44 +6192,41 @@
       <c r="H11" s="21">
         <v>13</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="29">
         <v>50</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="29">
         <v>6</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="L11" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="M11" s="28" t="s">
+      <c r="M11" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="N11" s="28" t="s">
+      <c r="N11" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="O11" s="28">
+      <c r="O11" s="29">
         <v>20</v>
       </c>
       <c r="Q11" s="28">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="R11" s="28">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S11" s="28" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="T11" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U11" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="V11" s="28">
+        <v>66</v>
+      </c>
+      <c r="U11" s="28">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:22">
+    <row r="12" spans="2:28">
       <c r="E12" s="29">
         <v>200</v>
       </c>
@@ -6044,25 +6258,22 @@
         <v>20</v>
       </c>
       <c r="Q12" s="28">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="R12" s="28">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="S12" s="28" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="T12" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U12" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="V12" s="28">
+        <v>89</v>
+      </c>
+      <c r="U12" s="28">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:22">
+    <row r="13" spans="2:28">
       <c r="E13" s="28">
         <v>220</v>
       </c>
@@ -6094,25 +6305,22 @@
         <v>25</v>
       </c>
       <c r="Q13" s="28">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="R13" s="28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S13" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T13" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U13" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="V13" s="28">
+        <v>88</v>
+      </c>
+      <c r="U13" s="28">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:22">
+    <row r="14" spans="2:28">
       <c r="E14" s="28">
         <v>240</v>
       </c>
@@ -6143,26 +6351,23 @@
       <c r="O14" s="28">
         <v>25</v>
       </c>
-      <c r="Q14" s="28">
-        <v>50</v>
-      </c>
-      <c r="R14" s="28">
-        <v>6</v>
-      </c>
-      <c r="S14" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="T14" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="U14" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="V14" s="28">
+      <c r="Q14" s="29">
+        <v>100</v>
+      </c>
+      <c r="R14" s="29">
+        <v>5</v>
+      </c>
+      <c r="S14" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="T14" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="U14" s="29">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:22">
+    <row r="15" spans="2:28">
       <c r="E15" s="28">
         <v>260</v>
       </c>
@@ -6175,44 +6380,41 @@
       <c r="H15" s="28">
         <v>13</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="31">
         <v>100</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="31">
         <v>4</v>
       </c>
-      <c r="L15" s="29" t="s">
+      <c r="L15" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="M15" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="N15" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="O15" s="29">
+      <c r="M15" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="N15" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="O15" s="31">
         <v>20</v>
       </c>
-      <c r="Q15" s="29">
+      <c r="Q15" s="28">
         <v>100</v>
       </c>
-      <c r="R15" s="29">
-        <v>4</v>
-      </c>
-      <c r="S15" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="T15" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U15" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="V15" s="29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22">
+      <c r="R15" s="28">
+        <v>10</v>
+      </c>
+      <c r="S15" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="T15" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="U15" s="31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28">
       <c r="E16" s="28">
         <v>300</v>
       </c>
@@ -6247,22 +6449,19 @@
         <v>100</v>
       </c>
       <c r="R16" s="28">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="S16" s="28" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="T16" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="U16" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="V16" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="5:22">
+        <v>89</v>
+      </c>
+      <c r="U16" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="5:21">
       <c r="E17" s="28">
         <v>400</v>
       </c>
@@ -6297,22 +6496,19 @@
         <v>100</v>
       </c>
       <c r="R17" s="28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S17" s="28" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="T17" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U17" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="V17" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="5:22">
+        <v>88</v>
+      </c>
+      <c r="U17" s="28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="5:21">
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
@@ -6335,25 +6531,22 @@
         <v>25</v>
       </c>
       <c r="Q18" s="28">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="R18" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S18" s="28" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="T18" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U18" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="V18" s="28">
+        <v>88</v>
+      </c>
+      <c r="U18" s="28">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="5:22">
+    <row r="19" spans="5:21">
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
@@ -6375,26 +6568,13 @@
       <c r="O19" s="28">
         <v>20</v>
       </c>
-      <c r="Q19" s="28">
-        <v>200</v>
-      </c>
-      <c r="R19" s="28">
-        <v>4</v>
-      </c>
-      <c r="S19" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="T19" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U19" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="V19" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="5:22">
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+    </row>
+    <row r="20" spans="5:21">
       <c r="J20" s="28">
         <v>200</v>
       </c>
@@ -6413,26 +6593,13 @@
       <c r="O20" s="28">
         <v>25</v>
       </c>
-      <c r="Q20" s="28">
-        <v>200</v>
-      </c>
-      <c r="R20" s="28">
-        <v>6</v>
-      </c>
-      <c r="S20" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="T20" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U20" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="V20" s="28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="5:22">
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+    </row>
+    <row r="21" spans="5:21">
       <c r="J21" s="28">
         <v>300</v>
       </c>
@@ -6451,26 +6618,13 @@
       <c r="O21" s="28">
         <v>20</v>
       </c>
-      <c r="Q21" s="28">
-        <v>300</v>
-      </c>
-      <c r="R21" s="28">
-        <v>4</v>
-      </c>
-      <c r="S21" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="T21" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U21" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="V21" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="5:22">
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+    </row>
+    <row r="22" spans="5:21">
       <c r="J22" s="28">
         <v>400</v>
       </c>
@@ -6489,29 +6643,17 @@
       <c r="O22" s="28">
         <v>20</v>
       </c>
-      <c r="Q22" s="28">
-        <v>400</v>
-      </c>
-      <c r="R22" s="28">
-        <v>4</v>
-      </c>
-      <c r="S22" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="T22" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U22" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="V22" s="28">
-        <v>20</v>
-      </c>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="J2:O2"/>
+    <mergeCell ref="Q2:U2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>